<commit_message>
Added Use Case Column
</commit_message>
<xml_diff>
--- a/BurpSuite_Extensions.xlsx
+++ b/BurpSuite_Extensions.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\getch\Documents\GitHub\Application-Pentest-Methodology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4E2211-17CC-49DD-A42A-8054FDAB813C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E82E3E8-96EB-4DBE-A921-041E8C6918F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BurpSuite Extensions" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'BurpSuite Extensions'!$A$1:$E$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'BurpSuite Extensions'!$A$1:$F$65</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="174">
   <si>
     <t>BurpSuite Extensions</t>
   </si>
@@ -459,6 +459,120 @@
   </si>
   <si>
     <t>The lazy-testers best friend. Allows for pasting into requests of common payloads such as XSS, SQLi, LFI, XXE, webshells, and revshells</t>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>User Interface Improvement</t>
+  </si>
+  <si>
+    <t>Automated Scanner Improvement</t>
+  </si>
+  <si>
+    <t>Obfuscation Support</t>
+  </si>
+  <si>
+    <t>Repeater Extender</t>
+  </si>
+  <si>
+    <t>RBAC Automation</t>
+  </si>
+  <si>
+    <t>Logger</t>
+  </si>
+  <si>
+    <t>CSRF Detection</t>
+  </si>
+  <si>
+    <t>Payload Generator</t>
+  </si>
+  <si>
+    <t>Cloud Security Checks</t>
+  </si>
+  <si>
+    <t>SSI Detection</t>
+  </si>
+  <si>
+    <t>OOB Detection</t>
+  </si>
+  <si>
+    <t>OS Command Injection Detection</t>
+  </si>
+  <si>
+    <t>CSP Vulnerability Checks</t>
+  </si>
+  <si>
+    <t>JavaScript Analysis</t>
+  </si>
+  <si>
+    <t>Outdated Software Detection</t>
+  </si>
+  <si>
+    <t>Log4Shell Detection</t>
+  </si>
+  <si>
+    <t>JWT Analysis</t>
+  </si>
+  <si>
+    <t>SSO Analysis</t>
+  </si>
+  <si>
+    <t>Metadata Analysis</t>
+  </si>
+  <si>
+    <t>File Upload Checks</t>
+  </si>
+  <si>
+    <t>Deserialization Checks</t>
+  </si>
+  <si>
+    <t>SOME Checker</t>
+  </si>
+  <si>
+    <t>SAML Checker</t>
+  </si>
+  <si>
+    <t>SOAP Analysis</t>
+  </si>
+  <si>
+    <t>Manual Exploit Assistor</t>
+  </si>
+  <si>
+    <t>Error Message Analysis</t>
+  </si>
+  <si>
+    <t>Header Analysis</t>
+  </si>
+  <si>
+    <t>HTTP Request Smuggling Checker</t>
+  </si>
+  <si>
+    <t>Hash Exploitation</t>
+  </si>
+  <si>
+    <t>Parameter Analysis</t>
+  </si>
+  <si>
+    <t>PHP Object Injection Checker</t>
+  </si>
+  <si>
+    <t>Reflected File Download Checkerer</t>
+  </si>
+  <si>
+    <t>Reverse Proxy Detection</t>
+  </si>
+  <si>
+    <t>SSL/TLS Analysis</t>
+  </si>
+  <si>
+    <t>Web Caching Checks</t>
+  </si>
+  <si>
+    <t>JWT Editor</t>
+  </si>
+  <si>
+    <t>Used for editing, signing, verifying, encrypting and decrypting JSON Web Tokens (JWTs).</t>
   </si>
 </sst>
 </file>
@@ -523,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -534,6 +648,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,16 +725,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E64" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:E64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D62">
-    <sortCondition ref="A1:A62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F65" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:F65" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D63">
+    <sortCondition ref="A1:A63"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="BurpSuite Extensions" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Pro?" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A Must install?"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Requires Configuration?"/>
+    <tableColumn id="6" xr3:uid="{C74299DC-E0EF-447A-82C9-B99AE1E6BFD6}" name="Use Case"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -923,23 +1039,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="175" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="6" max="6" width="175" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -952,11 +1069,14 @@
       <c r="D1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -967,10 +1087,13 @@
         <v>69</v>
       </c>
       <c r="E2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -984,10 +1107,13 @@
         <v>69</v>
       </c>
       <c r="E3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1001,10 +1127,13 @@
         <v>69</v>
       </c>
       <c r="E4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1018,10 +1147,13 @@
         <v>69</v>
       </c>
       <c r="E5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1031,11 +1163,14 @@
       <c r="D6" t="s">
         <v>69</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1046,10 +1181,13 @@
         <v>69</v>
       </c>
       <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1060,10 +1198,13 @@
         <v>69</v>
       </c>
       <c r="E8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1077,10 +1218,13 @@
         <v>69</v>
       </c>
       <c r="E9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>130</v>
       </c>
@@ -1091,10 +1235,13 @@
         <v>64</v>
       </c>
       <c r="E10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1108,10 +1255,13 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1122,10 +1272,13 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1136,10 +1289,13 @@
         <v>69</v>
       </c>
       <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -1153,10 +1309,13 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1170,10 +1329,13 @@
         <v>69</v>
       </c>
       <c r="E15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -1184,10 +1346,13 @@
         <v>69</v>
       </c>
       <c r="E16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1198,10 +1363,13 @@
         <v>69</v>
       </c>
       <c r="E17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1212,10 +1380,13 @@
         <v>69</v>
       </c>
       <c r="E18" t="s">
+        <v>140</v>
+      </c>
+      <c r="F18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -1226,10 +1397,13 @@
         <v>69</v>
       </c>
       <c r="E19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -1243,10 +1417,13 @@
         <v>69</v>
       </c>
       <c r="E20" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
@@ -1260,10 +1437,13 @@
         <v>69</v>
       </c>
       <c r="E21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1274,10 +1454,13 @@
         <v>69</v>
       </c>
       <c r="E22" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -1291,10 +1474,13 @@
         <v>69</v>
       </c>
       <c r="E23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1305,10 +1491,13 @@
         <v>64</v>
       </c>
       <c r="E24" t="s">
+        <v>154</v>
+      </c>
+      <c r="F24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>79</v>
       </c>
@@ -1319,10 +1508,13 @@
         <v>69</v>
       </c>
       <c r="E25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F25" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>80</v>
       </c>
@@ -1333,10 +1525,13 @@
         <v>69</v>
       </c>
       <c r="E26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>82</v>
       </c>
@@ -1347,10 +1542,13 @@
         <v>69</v>
       </c>
       <c r="E27" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -1364,10 +1562,13 @@
         <v>69</v>
       </c>
       <c r="E28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>120</v>
       </c>
@@ -1378,10 +1579,13 @@
         <v>64</v>
       </c>
       <c r="E29" t="s">
+        <v>157</v>
+      </c>
+      <c r="F29" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>134</v>
       </c>
@@ -1392,10 +1596,13 @@
         <v>69</v>
       </c>
       <c r="E30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -1409,10 +1616,13 @@
         <v>69</v>
       </c>
       <c r="E31" t="s">
+        <v>163</v>
+      </c>
+      <c r="F31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>26</v>
       </c>
@@ -1426,10 +1636,13 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F32" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>27</v>
       </c>
@@ -1440,10 +1653,13 @@
         <v>69</v>
       </c>
       <c r="E33" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>28</v>
       </c>
@@ -1454,10 +1670,13 @@
         <v>69</v>
       </c>
       <c r="E34" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>29</v>
       </c>
@@ -1471,10 +1690,13 @@
         <v>69</v>
       </c>
       <c r="E35" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>31</v>
       </c>
@@ -1488,10 +1710,13 @@
         <v>64</v>
       </c>
       <c r="E36" t="s">
+        <v>157</v>
+      </c>
+      <c r="F36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>32</v>
       </c>
@@ -1502,10 +1727,13 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
+        <v>157</v>
+      </c>
+      <c r="F37" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>33</v>
       </c>
@@ -1516,10 +1744,13 @@
         <v>69</v>
       </c>
       <c r="E38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>123</v>
       </c>
@@ -1530,10 +1761,13 @@
         <v>69</v>
       </c>
       <c r="E39" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1544,10 +1778,13 @@
         <v>69</v>
       </c>
       <c r="E40" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>35</v>
       </c>
@@ -1558,367 +1795,456 @@
         <v>3</v>
       </c>
       <c r="E41" t="s">
+        <v>153</v>
+      </c>
+      <c r="F41" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>36</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C42" t="s">
-        <v>3</v>
-      </c>
       <c r="D42" t="s">
         <v>64</v>
       </c>
       <c r="E42" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" t="s">
+        <v>153</v>
+      </c>
+      <c r="F43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="B44" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B45" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="B46" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" t="s">
+        <v>144</v>
+      </c>
+      <c r="F46" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46" t="s">
-        <v>69</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="B47" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C47" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="B48" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" t="s">
+        <v>166</v>
+      </c>
+      <c r="F48" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="B49" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>166</v>
+      </c>
+      <c r="F49" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="B50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" t="s">
+        <v>167</v>
+      </c>
+      <c r="F50" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>114</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C50" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="B51" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
         <v>115</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
+        <v>168</v>
+      </c>
+      <c r="F51" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="B52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" t="s">
+        <v>166</v>
+      </c>
+      <c r="F52" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="B53" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="B54" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F54" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>46</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" t="s">
-        <v>69</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="B55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" t="s">
+        <v>151</v>
+      </c>
+      <c r="F55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D55" t="s">
-        <v>69</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="B56" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" t="s">
+        <v>169</v>
+      </c>
+      <c r="F56" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="B57" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>69</v>
+      </c>
+      <c r="E57" t="s">
+        <v>158</v>
+      </c>
+      <c r="F57" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2" t="s">
+      <c r="B58" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="B59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>69</v>
+      </c>
+      <c r="E59" t="s">
+        <v>151</v>
+      </c>
+      <c r="F59" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" t="s">
-        <v>69</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="B60" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" t="s">
+        <v>151</v>
+      </c>
+      <c r="F60" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D60" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="B61" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>170</v>
+      </c>
+      <c r="F61" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E61" s="2" t="s">
+      <c r="B62" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B62" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="B63" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
         <v>64</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
+        <v>156</v>
+      </c>
+      <c r="F63" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>51</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" t="s">
-        <v>69</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="B64" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" t="s">
+        <v>171</v>
+      </c>
+      <c r="F64" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D64" t="s">
-        <v>69</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="B65" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" t="s">
+        <v>160</v>
+      </c>
+      <c r="F65" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>117</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D62">
-    <sortCondition ref="C2:C62"/>
-    <sortCondition ref="A2:A62"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D63">
+    <sortCondition ref="C2:C63"/>
+    <sortCondition ref="A2:A63"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1929,6 +2255,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="16903ae7-d79f-4213-82d3-72b247f98af7">
+      <UserInfo>
+        <DisplayName>Rodriguez, Angel</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F306FAD7936F2C44925D685513323D7F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="439575adb43509399c9be3e4511a3495">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16903ae7-d79f-4213-82d3-72b247f98af7" xmlns:ns3="5bb858cb-a0b9-45df-8671-22523941b482" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e307ae8063916f52b9ebba6b67d8c66" ns2:_="" ns3:_="">
     <xsd:import namespace="16903ae7-d79f-4213-82d3-72b247f98af7"/>
@@ -2139,20 +2479,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="16903ae7-d79f-4213-82d3-72b247f98af7">
-      <UserInfo>
-        <DisplayName>Rodriguez, Angel</DisplayName>
-        <AccountId>14</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2163,6 +2489,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{882978BD-D0D0-42FB-B17D-D7067E4B527C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="16903ae7-d79f-4213-82d3-72b247f98af7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2BAA58E-B6BE-4624-8B66-0279875543D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2181,16 +2517,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{882978BD-D0D0-42FB-B17D-D7067E4B527C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="16903ae7-d79f-4213-82d3-72b247f98af7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{497AE595-EED7-436F-8FDB-FA589B049D52}">
   <ds:schemaRefs>

</xml_diff>